<commit_message>
mode 1 release 2 and 3 analsyis
</commit_message>
<xml_diff>
--- a/Human_Evaluation/Data/Mode1/Analysis/mode_1_release_1_manual_test_evaluation.xlsx
+++ b/Human_Evaluation/Data/Mode1/Analysis/mode_1_release_1_manual_test_evaluation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkang/Documents/research/nlp_followupqg/Human_Evaluation/Data/Mode1/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7076CE1-1978-4448-BEDC-943FF6BB7A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853B9C0C-88EB-EE40-8C1B-6D7C1EC52A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18020" yWindow="-28300" windowWidth="25600" windowHeight="28300" xr2:uid="{6FD07B90-3C0D-B44C-9423-DFBC99719B27}"/>
   </bookViews>
@@ -418,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A0DB99-78D8-B044-BB14-062E960FDBAB}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -459,11 +459,8 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -479,11 +476,8 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -499,11 +493,8 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -519,11 +510,8 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -539,11 +527,8 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -559,11 +544,8 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -579,11 +561,8 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -599,11 +578,8 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -619,11 +595,8 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -638,9 +611,6 @@
       </c>
       <c r="E11">
         <v>1</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>